<commit_message>
finalized error estimates for annulus counts
</commit_message>
<xml_diff>
--- a/growth_analysis/data/otolith_recounts/michael_recount.xlsx
+++ b/growth_analysis/data/otolith_recounts/michael_recount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/growth_analysis/data/otolith_recounts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8890A5D9-04B6-D24C-AE60-0A9A32610A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CE701A-1730-D644-8334-DB64F6FA258C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34800" yWindow="1460" windowWidth="27060" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,13 +60,13 @@
     <t>FER54</t>
   </si>
   <si>
-    <t>FER60 </t>
-  </si>
-  <si>
     <t>FER62</t>
   </si>
   <si>
     <t>FER70</t>
+  </si>
+  <si>
+    <t>FER60</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="36" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -491,7 +491,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>3</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>

</xml_diff>